<commit_message>
Update evidence format error
</commit_message>
<xml_diff>
--- a/BCSungjin/evidence.xlsx
+++ b/BCSungjin/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="20"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Info"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="86">
   <si>
     <t>TxHash</t>
   </si>
@@ -55,25 +55,25 @@
     <t>63428F201BBB7EBCB76DD9B01B9AAC75D7B9454C1173EBF0C753836990FF3159</t>
   </si>
   <si>
-    <t>iris</t>
+    <t>gon-irishub-1</t>
   </si>
   <si>
     <t>E0205581556865EE1A9C229DB70A5E930A034FDD4CF2965DBE8930F9F23A3186</t>
   </si>
   <si>
-    <t>uptick</t>
+    <t>uptick_7000-2</t>
   </si>
   <si>
     <t>872F70CB4A48D8A3957D518FF1E7DC826FC2FC9C142C87BF9CC18C607B61D039</t>
   </si>
   <si>
-    <t>stargaze</t>
+    <t>elgafar-1</t>
   </si>
   <si>
     <t>6479081D252A3E452C3AAF2F45056D6CD2EADC61D3E8DAA9B580E0668547B2AF</t>
   </si>
   <si>
-    <t>omniflix</t>
+    <t>gon-flixnet-1</t>
   </si>
   <si>
     <t>CA3693A6E4DFA5848099B6B92DD202D5CBBE92116B35099CDBA21542E13EE488</t>
@@ -91,7 +91,7 @@
     <t>F08F4A9F2750833426E77B1B0AF15E7E27FDE052D68DB695E35F2C678515ADF4</t>
   </si>
   <si>
-    <t>juno</t>
+    <t>uni-6</t>
   </si>
   <si>
     <t>B3A4E0D05AF13975B9F533DEF4C96D6D3DA203BF5DF9F0E6EE9FDFCD5680D37C</t>
@@ -217,37 +217,37 @@
     <t>nftrune</t>
   </si>
   <si>
-    <t>0C9E50C4418196E24D9A49B6985140EE713336DD8AA48937C5EC472CB2329539</t>
+    <t>4C1F882C0E490E4B35BF104FFE64EF255D86417C930AD5EC16795564D45589ED</t>
   </si>
   <si>
     <t>ibc/CBF033AAC9F6CD6D56BA5C6779ADE9D2186A97BF8861F4DFA4DDE9F8A0BE443B</t>
   </si>
   <si>
-    <t>nftrune2</t>
-  </si>
-  <si>
-    <t>BFA4CF05513055CACDBDE3549C4731C9CB4C8F496A0CF0D6D8E54EF37277A5E3</t>
-  </si>
-  <si>
-    <t>stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh</t>
-  </si>
-  <si>
-    <t>3C43C11B93C4D17B238159E65CC44CE3052916E62734784BBB8A85D02DFD8B3B</t>
-  </si>
-  <si>
-    <t>F204A60CF9BCAFEF583B46FA9709392999AC618BD372B9AACD93E336725C7A6B</t>
+    <t>nnnftruneA4</t>
+  </si>
+  <si>
+    <t>F1C648889CE252A9CD2EDF9FC8162F5F9D8C5F77EFAE4277E14B386820FD674C</t>
   </si>
   <si>
     <t>stars1tnu6msyzdppvjym7uew6n69tg77pdrcyww5ppv6ymkn0l5wu26hq0t7hx5</t>
   </si>
   <si>
-    <t>1. 5D78A74E013013846A9F547561FB00920267FB263B8DCBFDAE87C95BB06E9CDF, 2.2961BF0C5D51939B42EABE78022E299537882B9286DC002459FF0F4C27A7E2AE</t>
+    <t>nnnftruneA3</t>
+  </si>
+  <si>
+    <t>11051C011690C9F9371739295F794A9F75F384AE6F003FB1043090F446981BF3</t>
+  </si>
+  <si>
+    <t>78A816372C0A34907D0004F190D0979914289E685EE25D3CB79E74DBE06CC0D5</t>
+  </si>
+  <si>
+    <t>034F5E21954632016AD2A297E7B8578F8153C1451E6A10A885779AC1A77A912A</t>
   </si>
   <si>
     <t>runeterra</t>
   </si>
   <si>
-    <t>nftrune, nftrune2</t>
+    <t>9ED64C8F9482791DA5EA2438C1BD89841039E6FB30501B9CB96ECC04C1F8AB4E</t>
   </si>
   <si>
     <t>D7C272323BBEAEE0B1F4207EC7BF31B4CE65A9EE3EF77593662C709EA5EB8E76</t>
@@ -303,7 +303,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -315,6 +315,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -384,7 +390,7 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -885,7 +891,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="20.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="87.43357142857143" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -921,8 +927,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="33.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="25.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="84.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -982,7 +988,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="3" width="83.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="9.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -1042,7 +1048,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="3" width="83.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -1102,7 +1108,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="3" width="83.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -1162,7 +1168,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="3" width="85.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -1222,7 +1228,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="3" width="83.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -1318,7 +1324,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="3" width="85.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -1389,12 +1395,12 @@
   </sheetPr>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="3" width="83.7192857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -1599,18 +1605,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="3" width="97.005" customWidth="1" bestFit="1"/>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="84.14785714285713" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="3" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="16.005" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <col min="3" max="3" style="3" width="17.719285714285714" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1629,8 +1635,19 @@
         <v>68</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="A3" s="2" t="s">
         <v>69</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1649,7 +1666,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="3" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="75.14785714285713" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="3" width="16.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
@@ -1670,13 +1687,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>9</v>
@@ -1699,12 +1716,62 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="3" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="89.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="15.43357142857143" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="75.14785714285713" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="3" width="16.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1718,9 +1785,59 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>64</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="54.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="3" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="3" width="15.43357142857143" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>60</v>
@@ -1737,106 +1854,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="3" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="3" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="3" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="3" width="14.43357142857143" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
@@ -1880,12 +1897,12 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="3" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="13.290714285714287" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">

</xml_diff>

<commit_message>
add evidence Task B1,B2
</commit_message>
<xml_diff>
--- a/BCSungjin/evidence.xlsx
+++ b/BCSungjin/evidence.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="8"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Info"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="90">
   <si>
     <t>TxHash</t>
   </si>
@@ -47,6 +47,18 @@
   </si>
   <si>
     <t>The Internal Transfer TxHash on IRISnet</t>
+  </si>
+  <si>
+    <t>56DA2318BEB0EEECD3AD3417043C3E42D0F36FB642978ADFF0997A000555A478</t>
+  </si>
+  <si>
+    <t>B93384F448A8A78FF622052132D80088BFE502A52CD4D77F6480CDFEA352DACB</t>
+  </si>
+  <si>
+    <t>18D4EF71AFD796892AE98E2C7BEBF269C4B881F1A2E18FFFE4F261B9248B835D</t>
+  </si>
+  <si>
+    <t>75DF57E16794FA3B0E40634C8225B6B9D35E63CDD8E5F7DCC98566130CD1E5FF</t>
   </si>
   <si>
     <t>ChainID</t>
@@ -319,7 +331,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -719,51 +731,51 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>75</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="7" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="H2" s="4"/>
     </row>
@@ -789,10 +801,82 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
@@ -808,7 +892,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -819,16 +903,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="87.43357142857143" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
@@ -844,78 +928,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="3" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="3" width="87.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
@@ -936,7 +948,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+      <c r="A4" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
+      <c r="A5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="83.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.862142857142858" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
@@ -944,7 +1016,7 @@
         <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
@@ -952,15 +1024,15 @@
         <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
@@ -968,15 +1040,15 @@
         <v>44</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -996,7 +1068,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
@@ -1004,7 +1076,7 @@
         <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
@@ -1012,7 +1084,7 @@
         <v>38</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
@@ -1028,43 +1100,43 @@
         <v>40</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="83.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="3" width="83.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="14.862142857142858" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
@@ -1072,15 +1144,15 @@
         <v>34</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
@@ -1088,15 +1160,15 @@
         <v>36</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -1107,7 +1179,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="83.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="85.29071428571429" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="6" width="14.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -1116,7 +1188,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
@@ -1124,7 +1196,7 @@
         <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
@@ -1132,7 +1204,7 @@
         <v>30</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
@@ -1140,7 +1212,7 @@
         <v>31</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
@@ -1148,15 +1220,15 @@
         <v>32</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -1167,8 +1239,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="85.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="14.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="3" width="83.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
@@ -1176,7 +1248,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
@@ -1184,7 +1256,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
@@ -1192,7 +1264,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
@@ -1200,7 +1272,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
@@ -1208,48 +1280,160 @@
         <v>28</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="17.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="17.862142857142857" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="85.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.862142857142858" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="3" width="83.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="14.862142857142858" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
+      <c r="A4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
+      <c r="A5" s="5" t="s">
         <v>22</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
+      <c r="A6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+      <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="83.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="14.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>11</v>
@@ -1257,165 +1441,62 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
       <c r="A4" s="5" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
-      <c r="A5" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="3" width="17.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="17.862142857142857" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="3" width="85.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="14.862142857142858" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
-      <c r="A4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
       <c r="A5" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
       <c r="A6" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="3" width="83.7192857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="14.576428571428572" customWidth="1" bestFit="1"/>
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="41.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.4">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1423,54 +1504,53 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18">
-      <c r="A4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18">
-      <c r="A5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18">
-      <c r="A6" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
-      <c r="A7" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
+    <sheetView workbookViewId="0" tabSelected="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="41.005" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1483,7 +1563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="16.4">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1498,7 +1578,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
@@ -1532,74 +1612,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
@@ -1621,32 +1633,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="2" t="s">
-        <v>67</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>68</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1671,32 +1683,32 @@
     <col min="4" max="4" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1726,27 +1738,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1776,27 +1788,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1826,13 +1838,91 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+      <c r="A2" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="3" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="13.290714285714287" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+      <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
@@ -1842,84 +1932,6 @@
       <c r="B2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="3" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="12.43357142857143" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="3" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.290714285714287" customWidth="1" bestFit="1"/>
-  </cols>
-  <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
-      <c r="A1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>56</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>